<commit_message>
Optimize the code for all features
</commit_message>
<xml_diff>
--- a/Parcel-Test-Features/Project-List-Grid/bin/Test_Data/Project_List_Grid_Feature.xlsx
+++ b/Parcel-Test-Features/Project-List-Grid/bin/Test_Data/Project_List_Grid_Feature.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -56,7 +56,7 @@
     <t>spatil</t>
   </si>
   <si>
-    <t>PCA test009</t>
+    <t>PCA test010</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>